<commit_message>
bump difficulties to 7
update example.xlsx accordingly
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="41">
   <si>
     <t>נושא אש</t>
   </si>
@@ -233,6 +233,128 @@
   </si>
   <si>
     <t>זה לא משנה תעצור את זה אח שלי</t>
+  </si>
+  <si>
+    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit</t>
+  </si>
+  <si>
+    <t>sed do eiusmod tempor incididunt ut labore</t>
+  </si>
+  <si>
+    <t>et dolore magna aliqua</t>
+  </si>
+  <si>
+    <t>Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat</t>
+  </si>
+  <si>
+    <t>Duis aute irure</t>
+  </si>
+  <si>
+    <t>dolor in reprehenderit in voluptate velit esse cillum dolore eu fugiat nulla pariatur. Excepteur sint</t>
+  </si>
+  <si>
+    <t>במפגש משפחתי אחד, צעיר אחד פנה להוריו, דודיו וסבותיו ושאל: כיצד יכולתם לחיות בעבר, ללא:</t>
+  </si>
+  <si>
+    <t>טכנולוגיה
+אינטרנט
+מחשבים
+מזלט”ים
+ביטקוין
+טחפונים סלולריים
+פייסבוק
+טוויטר
+ללא…
+ללא…</t>
+  </si>
+  <si>
+    <t>הסבא ענה לו, ובכן ראה נכדי היקר,
+בדיוק כמו הדור שלך שחי היום:
+ללא תפילה
+ללא כבוד
+ללא רגש
+ללא בושה
+ללא כיבוד הזולת
+ללא אופי
+ללא כבוד עצמי
+ללא צניעות…</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color indexed="11"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">אנו שנולדו בין השנים 1930-1980, אנו מבורכים, חיינו הנם דוגמא חיה.
+</t>
+    </r>
+  </si>
+  <si>
+    <t>אחרי ביה”ס 👈
+👈 עשינו שיעורים ויצאנו לרחוב לשחק!
+👈שיחקנו עם חברים אמיתיים, לא חברי אינטרנט…
+👈ידענו ליצור משחקים משלנו ולשחק בהם.
+👈הורינו לא היו עשירים, אך העניקו לנו אהבה ולא חפצים ארציים.
+👈מעולם לא היו לנו טלפונים סלולריים, DVD, פלייסטיישן, XBOX, משחקי ווידאו, מחשבים אישיים, אינטרנט… אך היו לנו חברים אמיתיים.
+👈בני המשפחה גרו קרוב כדי ליהנות מהזמן בקרבת המשפחה.
+👈אמנם הופענו בתצלומים בשחור לבן, אך תוכל למצוא הרבה זכרונות צבעוניים בתמונות הללו.
+👈אנו דור ייחודי ואחרון שהקשיב להוריו…
+👈 וגם הראשונים שנאלצים להקשיב לילדינו…</t>
+  </si>
+  <si>
+    <t>אנו גירסה מוגבלת בזמן ובמקום. נצל את היותנו והערך אותנו, למד מאיתנו והעבר זאת לחבריך.
+פוסט ספרדי שתורגם לעברית</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color indexed="11"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">עם קצת מעל 130 IQ אני חושב שיש לי את היכולת הקוגנטיבית להבין הומור אבסורדיסטי, ולהבחין בטונים אקזיסטנציאליזטים או ניהיליסטים.
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color indexed="11"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">אז לא, אני לא “פשוט לא מבין את הסדרה”. ריק ומורטי היא פשוט סדרה בינונית, פשטנית, עם מוטיב אחד ברור וחוזר, שאין בו שום עומק מיוחד, וההומור בה אבסורדי ומהנה אבל ממש לא גאוני ומתוחכם.
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color indexed="11"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">כל העומק הפילוסופי שאנשים רואים בה זה רצון כנה להאמין שזה מצחיק כי זה חכם ולא שזה מצחיק, על אף שזה לא מאוד חכם.
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color indexed="11"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">בחיי, נמאס לי לשמוע על זה. אם משברים אקזיסטנציאליסטים וניהיליזם זה באמת מה שאתם מחפים, תקראו ספרות רוסית פור פאק סייק.
+</t>
+    </r>
+  </si>
+  <si>
+    <t>למען ההגינות, יש צורך במנת משכל גבוהה ביותר בכדי להבין את ריק ומורטי</t>
+  </si>
+  <si>
+    <t>ההומור מעודן בטירוף, וללא הבנה חזקה של פיזיקה תאורטית הבדיחות שם פשוט תחלופנה מעל ראשו של הצופה הטיפוסי</t>
   </si>
 </sst>
 </file>
@@ -242,7 +364,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -268,6 +390,11 @@
       <sz val="16"/>
       <color indexed="11"/>
       <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="26"/>
+      <color indexed="12"/>
+      <name val="Georgia"/>
     </font>
   </fonts>
   <fills count="3">
@@ -313,7 +440,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -336,9 +463,18 @@
       <alignment horizontal="right" vertical="bottom" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" readingOrder="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -364,6 +500,7 @@
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ff212529"/>
+      <rgbColor rgb="ff7b8898"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1434,7 +1571,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6667" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="37.4609" style="1" customWidth="1"/>
+    <col min="1" max="1" width="37.5" style="1" customWidth="1"/>
     <col min="2" max="6" width="12.6719" style="1" customWidth="1"/>
     <col min="7" max="16384" width="12.6719" style="1" customWidth="1"/>
   </cols>
@@ -1475,7 +1612,7 @@
       <c r="E2" t="s" s="6">
         <v>10</v>
       </c>
-      <c r="F2" t="s" s="8">
+      <c r="F2" t="s" s="7">
         <v>11</v>
       </c>
     </row>
@@ -1483,7 +1620,7 @@
       <c r="A3" t="s" s="6">
         <v>12</v>
       </c>
-      <c r="B3" t="s" s="8">
+      <c r="B3" t="s" s="7">
         <v>13</v>
       </c>
       <c r="C3" t="s" s="6">
@@ -1495,7 +1632,7 @@
       <c r="E3" t="s" s="6">
         <v>16</v>
       </c>
-      <c r="F3" t="s" s="8">
+      <c r="F3" t="s" s="7">
         <v>11</v>
       </c>
     </row>
@@ -1515,57 +1652,93 @@
       <c r="E4" t="s" s="6">
         <v>21</v>
       </c>
-      <c r="F4" t="s" s="4">
+      <c r="F4" t="s" s="3">
         <v>22</v>
       </c>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="A5" t="s" s="4">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s" s="8">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s" s="4">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s" s="4">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s" s="4">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s" s="4">
+        <v>28</v>
+      </c>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
+      <c r="A6" t="s" s="4">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s" s="7">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s" s="7">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s" s="10">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s" s="7">
+        <v>33</v>
+      </c>
+      <c r="F6" t="s" s="7">
+        <v>34</v>
+      </c>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
+      <c r="A7" t="s" s="10">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s" s="11">
+        <v>36</v>
+      </c>
+      <c r="C7" t="s" s="10">
+        <v>37</v>
+      </c>
+      <c r="D7" t="s" s="10">
+        <v>38</v>
+      </c>
+      <c r="E7" t="s" s="4">
+        <v>39</v>
+      </c>
+      <c r="F7" t="s" s="4">
+        <v>40</v>
+      </c>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>

<commit_message>
example.xlsx add another row
now it's actually 7
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="47">
   <si>
     <t>נושא אש</t>
   </si>
@@ -355,6 +355,24 @@
   </si>
   <si>
     <t>ההומור מעודן בטירוף, וללא הבנה חזקה של פיזיקה תאורטית הבדיחות שם פשוט תחלופנה מעל ראשו של הצופה הטיפוסי</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> גם התפיסה הניהיליסטית של ריק, שקשורה באופן הדוק לאופיו – הפילוסופיה האישית שלו קיבלה השראה מאוד עמוקה מספרותה של “נרדוניה ווליה”, לדוגמה</t>
+  </si>
+  <si>
+    <t>המעריצים מבינים את הדברים הללו</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> להם את היכולת האינטלקטואלית להעריך באמת את עומק הבדיחות, להבין שהן לא סתם מצחיקות – הן אומרות משהו עמוק על החיים</t>
+  </si>
+  <si>
+    <t>כתוצאה מכך, אנשים שלא אוהבים את ריק ומורטי הם באמת אידיוטים</t>
+  </si>
+  <si>
+    <t>ברור שהם לא יעריכו, לדוגמה, את ההומור בביטוי הקליט האקזיסטנציאלי של ריק “וואבה לאבה דאב דאב”, שהוא בעצם רפרנס נסתר ל”אבות ובנים” של טורגנייב</t>
+  </si>
+  <si>
+    <t>אני מחייך כעת רק מלדמיין את הנבערים המשתאים מגרדים בראשם בבלבול אל מול גאונותו של דן הרמון הנפרשת מולם על מסכי הטלוויזיה. אילו כסילים… כמה אני מרחם עליהם. 😂 וכן, דרך אגב, אכן יש לי קעקוע של ריק ומורטי. ולא, אתם לא יכולים לראות אותו. הוא לעיני הבחורות בלבד – וגם הן צריכות להוכיח שהן בטווח 5 נקודות אייקיו משלי (עדיף כלפי מטה) לפני כן</t>
   </si>
 </sst>
 </file>
@@ -1717,12 +1735,24 @@
       </c>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
+      <c r="A8" t="s" s="4">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s" s="4">
+        <v>42</v>
+      </c>
+      <c r="C8" t="s" s="4">
+        <v>43</v>
+      </c>
+      <c r="D8" t="s" s="4">
+        <v>44</v>
+      </c>
+      <c r="E8" t="s" s="4">
+        <v>45</v>
+      </c>
+      <c r="F8" t="s" s="4">
+        <v>46</v>
+      </c>
     </row>
     <row r="9" ht="13.65" customHeight="1">
       <c r="A9" s="12"/>

</xml_diff>